<commit_message>
Adding use router refrence
</commit_message>
<xml_diff>
--- a/track.xlsx
+++ b/track.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mosta\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\dashboardv.4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90945FE0-2646-464F-9B24-DBBCE65F46E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5E2F17-1C9E-44FB-995D-03D781549AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,6 +19,7 @@
     <definedName name="Table3">Table6[]</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -1221,8 +1222,8 @@
   <dimension ref="A1:AJ72"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AH12" sqref="AH12"/>
+      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AH19" sqref="AH19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -1399,11 +1400,11 @@
       <c r="AH2" s="16"/>
       <c r="AI2" s="6">
         <f>(AI3+(AJ3/60))/60</f>
-        <v>0.45</v>
+        <v>0.7</v>
       </c>
       <c r="AJ2" s="7">
         <f>(AI3+(AJ3/60))</f>
-        <v>27</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.25">
@@ -1521,7 +1522,7 @@
       </c>
       <c r="AI3" s="8">
         <f>SUMIF(Table57[CHECK],"Done",AI$4:AI$71)</f>
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="AJ3" s="8">
         <f>SUMIF(Table57[CHECK],"Done",AJ$4:AJ$71)</f>
@@ -1567,7 +1568,7 @@
       </c>
       <c r="M4" s="15">
         <f ca="1">TODAY()</f>
-        <v>45469</v>
+        <v>45471</v>
       </c>
       <c r="N4" s="1">
         <v>0</v>
@@ -1600,7 +1601,7 @@
       </c>
       <c r="Y4" s="15">
         <f ca="1">TODAY()</f>
-        <v>45469</v>
+        <v>45471</v>
       </c>
       <c r="Z4" s="1">
         <v>0</v>
@@ -1671,7 +1672,7 @@
       </c>
       <c r="M5" s="15">
         <f ca="1">M4+1</f>
-        <v>45470</v>
+        <v>45472</v>
       </c>
       <c r="N5" s="1">
         <v>2.0833333333333333E-3</v>
@@ -1705,7 +1706,7 @@
       </c>
       <c r="Y5" s="15">
         <f ca="1">Y4+1</f>
-        <v>45470</v>
+        <v>45472</v>
       </c>
       <c r="Z5" s="1">
         <v>1.0416666666666667E-3</v>
@@ -1775,7 +1776,7 @@
       </c>
       <c r="M6" s="15">
         <f t="shared" ref="M6:M69" ca="1" si="2">M5+1</f>
-        <v>45471</v>
+        <v>45473</v>
       </c>
       <c r="N6" s="1">
         <v>4.1666666666666701E-3</v>
@@ -1809,7 +1810,7 @@
       </c>
       <c r="Y6" s="15">
         <f t="shared" ref="Y6:Y61" ca="1" si="4">Y5+1</f>
-        <v>45471</v>
+        <v>45473</v>
       </c>
       <c r="Z6" s="1">
         <v>2.0833333333333298E-3</v>
@@ -1879,7 +1880,7 @@
       </c>
       <c r="M7" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45472</v>
+        <v>45474</v>
       </c>
       <c r="N7" s="1">
         <v>6.2500000000000003E-3</v>
@@ -1913,7 +1914,7 @@
       </c>
       <c r="Y7" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45472</v>
+        <v>45474</v>
       </c>
       <c r="Z7" s="1">
         <v>3.1250000000000002E-3</v>
@@ -1983,7 +1984,7 @@
       </c>
       <c r="M8" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45473</v>
+        <v>45475</v>
       </c>
       <c r="N8" s="1">
         <v>8.3333333333333297E-3</v>
@@ -2017,7 +2018,7 @@
       </c>
       <c r="Y8" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45473</v>
+        <v>45475</v>
       </c>
       <c r="Z8" s="1">
         <v>4.1666666666666701E-3</v>
@@ -2087,7 +2088,7 @@
       </c>
       <c r="M9" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45474</v>
+        <v>45476</v>
       </c>
       <c r="N9" s="1">
         <v>1.0416666666666701E-2</v>
@@ -2121,7 +2122,7 @@
       </c>
       <c r="Y9" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45474</v>
+        <v>45476</v>
       </c>
       <c r="Z9" s="1">
         <v>5.2083333333333296E-3</v>
@@ -2191,7 +2192,7 @@
       </c>
       <c r="M10" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45475</v>
+        <v>45477</v>
       </c>
       <c r="N10" s="1">
         <v>1.2500000000000001E-2</v>
@@ -2225,7 +2226,7 @@
       </c>
       <c r="Y10" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45475</v>
+        <v>45477</v>
       </c>
       <c r="Z10" s="1">
         <v>6.2500000000000003E-3</v>
@@ -2295,7 +2296,7 @@
       </c>
       <c r="M11" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45476</v>
+        <v>45478</v>
       </c>
       <c r="N11" s="1">
         <v>1.4583333333333301E-2</v>
@@ -2329,7 +2330,7 @@
       </c>
       <c r="Y11" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45476</v>
+        <v>45478</v>
       </c>
       <c r="Z11" s="1">
         <v>7.2916666666666703E-3</v>
@@ -2399,7 +2400,7 @@
       </c>
       <c r="M12" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45477</v>
+        <v>45479</v>
       </c>
       <c r="N12" s="1">
         <v>1.6666666666666701E-2</v>
@@ -2433,7 +2434,7 @@
       </c>
       <c r="Y12" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45477</v>
+        <v>45479</v>
       </c>
       <c r="Z12" s="1">
         <v>8.3333333333333297E-3</v>
@@ -2503,7 +2504,7 @@
       </c>
       <c r="M13" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45478</v>
+        <v>45480</v>
       </c>
       <c r="N13" s="1">
         <v>1.8749999999999999E-2</v>
@@ -2537,7 +2538,7 @@
       </c>
       <c r="Y13" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45478</v>
+        <v>45480</v>
       </c>
       <c r="Z13" s="1">
         <v>9.3749999999999997E-3</v>
@@ -2558,7 +2559,9 @@
       <c r="AG13" s="1">
         <v>2.0833333333333301E-2</v>
       </c>
-      <c r="AH13" s="10"/>
+      <c r="AH13" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="AI13" s="2">
         <v>3</v>
       </c>
@@ -2592,7 +2595,7 @@
       </c>
       <c r="M14" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45479</v>
+        <v>45481</v>
       </c>
       <c r="N14" s="1">
         <v>2.0833333333333301E-2</v>
@@ -2626,7 +2629,7 @@
       </c>
       <c r="Y14" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45479</v>
+        <v>45481</v>
       </c>
       <c r="Z14" s="1">
         <v>1.0416666666666701E-2</v>
@@ -2647,7 +2650,9 @@
       <c r="AG14" s="1">
         <v>2.29166666666667E-2</v>
       </c>
-      <c r="AH14" s="10"/>
+      <c r="AH14" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="AI14" s="2">
         <v>3</v>
       </c>
@@ -2681,7 +2686,7 @@
       </c>
       <c r="M15" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45480</v>
+        <v>45482</v>
       </c>
       <c r="N15" s="1">
         <v>2.29166666666667E-2</v>
@@ -2715,7 +2720,7 @@
       </c>
       <c r="Y15" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45480</v>
+        <v>45482</v>
       </c>
       <c r="Z15" s="1">
         <v>1.14583333333333E-2</v>
@@ -2736,7 +2741,9 @@
       <c r="AG15" s="1">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AH15" s="10"/>
+      <c r="AH15" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="AI15" s="2">
         <v>3</v>
       </c>
@@ -2770,7 +2777,7 @@
       </c>
       <c r="M16" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45481</v>
+        <v>45483</v>
       </c>
       <c r="N16" s="1">
         <v>2.5000000000000001E-2</v>
@@ -2804,7 +2811,7 @@
       </c>
       <c r="Y16" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45481</v>
+        <v>45483</v>
       </c>
       <c r="Z16" s="1">
         <v>1.2500000000000001E-2</v>
@@ -2825,7 +2832,9 @@
       <c r="AG16" s="1">
         <v>2.70833333333333E-2</v>
       </c>
-      <c r="AH16" s="10"/>
+      <c r="AH16" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="AI16" s="2">
         <v>3</v>
       </c>
@@ -2859,7 +2868,7 @@
       </c>
       <c r="M17" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45482</v>
+        <v>45484</v>
       </c>
       <c r="N17" s="1">
         <v>2.70833333333333E-2</v>
@@ -2893,7 +2902,7 @@
       </c>
       <c r="Y17" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45482</v>
+        <v>45484</v>
       </c>
       <c r="Z17" s="1">
         <v>1.35416666666667E-2</v>
@@ -2914,7 +2923,9 @@
       <c r="AG17" s="1">
         <v>2.9166666666666698E-2</v>
       </c>
-      <c r="AH17" s="10"/>
+      <c r="AH17" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="AI17" s="2">
         <v>3</v>
       </c>
@@ -2948,7 +2959,7 @@
       </c>
       <c r="M18" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45483</v>
+        <v>45485</v>
       </c>
       <c r="N18" s="1">
         <v>2.9166666666666698E-2</v>
@@ -2982,7 +2993,7 @@
       </c>
       <c r="Y18" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45483</v>
+        <v>45485</v>
       </c>
       <c r="Z18" s="1">
         <v>1.4583333333333301E-2</v>
@@ -3037,7 +3048,7 @@
       </c>
       <c r="M19" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45484</v>
+        <v>45486</v>
       </c>
       <c r="N19" s="1">
         <v>3.125E-2</v>
@@ -3071,7 +3082,7 @@
       </c>
       <c r="Y19" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45484</v>
+        <v>45486</v>
       </c>
       <c r="Z19" s="1">
         <v>1.5625E-2</v>
@@ -3126,7 +3137,7 @@
       </c>
       <c r="M20" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45485</v>
+        <v>45487</v>
       </c>
       <c r="N20" s="1">
         <v>3.3333333333333298E-2</v>
@@ -3160,7 +3171,7 @@
       </c>
       <c r="Y20" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45485</v>
+        <v>45487</v>
       </c>
       <c r="Z20" s="1">
         <v>1.6666666666666701E-2</v>
@@ -3215,7 +3226,7 @@
       </c>
       <c r="M21" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45486</v>
+        <v>45488</v>
       </c>
       <c r="N21" s="1">
         <v>3.54166666666667E-2</v>
@@ -3249,7 +3260,7 @@
       </c>
       <c r="Y21" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45486</v>
+        <v>45488</v>
       </c>
       <c r="Z21" s="1">
         <v>1.7708333333333302E-2</v>
@@ -3304,7 +3315,7 @@
       </c>
       <c r="M22" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45487</v>
+        <v>45489</v>
       </c>
       <c r="N22" s="1">
         <v>3.7499999999999999E-2</v>
@@ -3338,7 +3349,7 @@
       </c>
       <c r="Y22" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45487</v>
+        <v>45489</v>
       </c>
       <c r="Z22" s="1">
         <v>1.8749999999999999E-2</v>
@@ -3393,7 +3404,7 @@
       </c>
       <c r="M23" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45488</v>
+        <v>45490</v>
       </c>
       <c r="N23" s="1">
         <v>3.9583333333333297E-2</v>
@@ -3423,7 +3434,7 @@
       <c r="X23" s="2"/>
       <c r="Y23" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45488</v>
+        <v>45490</v>
       </c>
       <c r="Z23" s="1">
         <v>1.97916666666667E-2</v>
@@ -3478,7 +3489,7 @@
       </c>
       <c r="M24" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45489</v>
+        <v>45491</v>
       </c>
       <c r="N24" s="1">
         <v>4.1666666666666699E-2</v>
@@ -3508,7 +3519,7 @@
       <c r="X24" s="2"/>
       <c r="Y24" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45489</v>
+        <v>45491</v>
       </c>
       <c r="Z24" s="1">
         <v>2.0833333333333301E-2</v>
@@ -3552,7 +3563,7 @@
       <c r="L25" s="2"/>
       <c r="M25" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45490</v>
+        <v>45492</v>
       </c>
       <c r="N25" s="1">
         <v>4.3749999999999997E-2</v>
@@ -3582,7 +3593,7 @@
       <c r="X25" s="2"/>
       <c r="Y25" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45490</v>
+        <v>45492</v>
       </c>
       <c r="Z25" s="1">
         <v>2.1874999999999999E-2</v>
@@ -3626,7 +3637,7 @@
       <c r="L26" s="2"/>
       <c r="M26" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45491</v>
+        <v>45493</v>
       </c>
       <c r="N26" s="1">
         <v>4.5833333333333302E-2</v>
@@ -3656,7 +3667,7 @@
       <c r="X26" s="2"/>
       <c r="Y26" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45491</v>
+        <v>45493</v>
       </c>
       <c r="Z26" s="1">
         <v>2.29166666666667E-2</v>
@@ -3700,7 +3711,7 @@
       <c r="L27" s="2"/>
       <c r="M27" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45492</v>
+        <v>45494</v>
       </c>
       <c r="N27" s="1">
         <v>4.7916666666666698E-2</v>
@@ -3730,7 +3741,7 @@
       <c r="X27" s="2"/>
       <c r="Y27" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45492</v>
+        <v>45494</v>
       </c>
       <c r="Z27" s="1">
         <v>2.39583333333333E-2</v>
@@ -3774,7 +3785,7 @@
       <c r="L28" s="2"/>
       <c r="M28" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45493</v>
+        <v>45495</v>
       </c>
       <c r="N28" s="1">
         <v>0.05</v>
@@ -3804,7 +3815,7 @@
       <c r="X28" s="2"/>
       <c r="Y28" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45493</v>
+        <v>45495</v>
       </c>
       <c r="Z28" s="1">
         <v>2.5000000000000001E-2</v>
@@ -3848,7 +3859,7 @@
       <c r="L29" s="2"/>
       <c r="M29" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45494</v>
+        <v>45496</v>
       </c>
       <c r="N29" s="1">
         <v>5.2083333333333301E-2</v>
@@ -3878,7 +3889,7 @@
       <c r="X29" s="2"/>
       <c r="Y29" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45494</v>
+        <v>45496</v>
       </c>
       <c r="Z29" s="1">
         <v>2.6041666666666699E-2</v>
@@ -3922,7 +3933,7 @@
       <c r="L30" s="2"/>
       <c r="M30" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45495</v>
+        <v>45497</v>
       </c>
       <c r="N30" s="1">
         <v>5.4166666666666703E-2</v>
@@ -3952,7 +3963,7 @@
       <c r="X30" s="2"/>
       <c r="Y30" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45495</v>
+        <v>45497</v>
       </c>
       <c r="Z30" s="1">
         <v>2.70833333333333E-2</v>
@@ -3996,7 +4007,7 @@
       <c r="L31" s="2"/>
       <c r="M31" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45496</v>
+        <v>45498</v>
       </c>
       <c r="N31" s="1">
         <v>5.6250000000000001E-2</v>
@@ -4026,7 +4037,7 @@
       <c r="X31" s="2"/>
       <c r="Y31" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45496</v>
+        <v>45498</v>
       </c>
       <c r="Z31" s="1">
         <v>2.8125000000000001E-2</v>
@@ -4070,7 +4081,7 @@
       <c r="L32" s="2"/>
       <c r="M32" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45497</v>
+        <v>45499</v>
       </c>
       <c r="N32" s="1">
         <v>5.83333333333333E-2</v>
@@ -4100,7 +4111,7 @@
       <c r="X32" s="2"/>
       <c r="Y32" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45497</v>
+        <v>45499</v>
       </c>
       <c r="Z32" s="1">
         <v>2.9166666666666698E-2</v>
@@ -4144,7 +4155,7 @@
       <c r="L33" s="2"/>
       <c r="M33" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45498</v>
+        <v>45500</v>
       </c>
       <c r="N33" s="1">
         <v>6.0416666666666702E-2</v>
@@ -4174,7 +4185,7 @@
       <c r="X33" s="2"/>
       <c r="Y33" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45498</v>
+        <v>45500</v>
       </c>
       <c r="Z33" s="1">
         <v>3.0208333333333299E-2</v>
@@ -4218,7 +4229,7 @@
       <c r="L34" s="2"/>
       <c r="M34" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45499</v>
+        <v>45501</v>
       </c>
       <c r="N34" s="1">
         <v>6.25E-2</v>
@@ -4248,7 +4259,7 @@
       <c r="X34" s="2"/>
       <c r="Y34" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45499</v>
+        <v>45501</v>
       </c>
       <c r="Z34" s="1">
         <v>3.125E-2</v>
@@ -4292,7 +4303,7 @@
       <c r="L35" s="2"/>
       <c r="M35" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45500</v>
+        <v>45502</v>
       </c>
       <c r="N35" s="1">
         <v>6.4583333333333298E-2</v>
@@ -4322,7 +4333,7 @@
       <c r="X35" s="2"/>
       <c r="Y35" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45500</v>
+        <v>45502</v>
       </c>
       <c r="Z35" s="1">
         <v>3.2291666666666698E-2</v>
@@ -4366,7 +4377,7 @@
       <c r="L36" s="2"/>
       <c r="M36" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45501</v>
+        <v>45503</v>
       </c>
       <c r="N36" s="1">
         <v>6.6666666666666693E-2</v>
@@ -4396,7 +4407,7 @@
       <c r="X36" s="2"/>
       <c r="Y36" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45501</v>
+        <v>45503</v>
       </c>
       <c r="Z36" s="1">
         <v>3.3333333333333298E-2</v>
@@ -4440,7 +4451,7 @@
       <c r="L37" s="2"/>
       <c r="M37" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45502</v>
+        <v>45504</v>
       </c>
       <c r="N37" s="1">
         <v>6.8750000000000006E-2</v>
@@ -4470,7 +4481,7 @@
       <c r="X37" s="2"/>
       <c r="Y37" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45502</v>
+        <v>45504</v>
       </c>
       <c r="Z37" s="1">
         <v>3.4375000000000003E-2</v>
@@ -4514,7 +4525,7 @@
       <c r="L38" s="2"/>
       <c r="M38" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45503</v>
+        <v>45505</v>
       </c>
       <c r="N38" s="1">
         <v>7.0833333333333304E-2</v>
@@ -4544,7 +4555,7 @@
       <c r="X38" s="2"/>
       <c r="Y38" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45503</v>
+        <v>45505</v>
       </c>
       <c r="Z38" s="1">
         <v>3.54166666666667E-2</v>
@@ -4588,7 +4599,7 @@
       <c r="L39" s="2"/>
       <c r="M39" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45504</v>
+        <v>45506</v>
       </c>
       <c r="N39" s="1">
         <v>7.2916666666666699E-2</v>
@@ -4618,7 +4629,7 @@
       <c r="X39" s="2"/>
       <c r="Y39" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45504</v>
+        <v>45506</v>
       </c>
       <c r="Z39" s="1">
         <v>3.6458333333333301E-2</v>
@@ -4662,7 +4673,7 @@
       <c r="L40" s="2"/>
       <c r="M40" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45505</v>
+        <v>45507</v>
       </c>
       <c r="N40" s="1">
         <v>7.4999999999999997E-2</v>
@@ -4692,7 +4703,7 @@
       <c r="X40" s="2"/>
       <c r="Y40" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45505</v>
+        <v>45507</v>
       </c>
       <c r="Z40" s="1">
         <v>3.7499999999999999E-2</v>
@@ -4736,7 +4747,7 @@
       <c r="L41" s="2"/>
       <c r="M41" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45506</v>
+        <v>45508</v>
       </c>
       <c r="N41" s="1">
         <v>7.7083333333333295E-2</v>
@@ -4762,7 +4773,7 @@
       <c r="X41" s="2"/>
       <c r="Y41" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45506</v>
+        <v>45508</v>
       </c>
       <c r="Z41" s="1">
         <v>3.8541666666666703E-2</v>
@@ -4806,7 +4817,7 @@
       <c r="L42" s="2"/>
       <c r="M42" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45507</v>
+        <v>45509</v>
       </c>
       <c r="N42" s="1">
         <v>7.9166666666666705E-2</v>
@@ -4832,7 +4843,7 @@
       <c r="X42" s="2"/>
       <c r="Y42" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45507</v>
+        <v>45509</v>
       </c>
       <c r="Z42" s="1">
         <v>3.9583333333333297E-2</v>
@@ -4876,7 +4887,7 @@
       <c r="L43" s="2"/>
       <c r="M43" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45508</v>
+        <v>45510</v>
       </c>
       <c r="N43" s="1">
         <v>8.1250000000000003E-2</v>
@@ -4902,7 +4913,7 @@
       <c r="X43" s="2"/>
       <c r="Y43" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45508</v>
+        <v>45510</v>
       </c>
       <c r="Z43" s="1">
         <v>4.1666666666666664E-2</v>
@@ -4946,7 +4957,7 @@
       <c r="L44" s="2"/>
       <c r="M44" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45509</v>
+        <v>45511</v>
       </c>
       <c r="N44" s="1">
         <v>8.3333333333333301E-2</v>
@@ -4972,7 +4983,7 @@
       <c r="X44" s="2"/>
       <c r="Y44" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45509</v>
+        <v>45511</v>
       </c>
       <c r="Z44" s="1">
         <v>4.5833333333333302E-2</v>
@@ -5016,7 +5027,7 @@
       <c r="L45" s="2"/>
       <c r="M45" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45510</v>
+        <v>45512</v>
       </c>
       <c r="N45" s="1">
         <v>8.5416666666666696E-2</v>
@@ -5042,7 +5053,7 @@
       <c r="X45" s="2"/>
       <c r="Y45" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45510</v>
+        <v>45512</v>
       </c>
       <c r="Z45" s="1">
         <v>4.9999999999999899E-2</v>
@@ -5086,7 +5097,7 @@
       <c r="L46" s="2"/>
       <c r="M46" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45511</v>
+        <v>45513</v>
       </c>
       <c r="N46" s="1">
         <v>8.7499999999999994E-2</v>
@@ -5112,7 +5123,7 @@
       <c r="X46" s="2"/>
       <c r="Y46" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45511</v>
+        <v>45513</v>
       </c>
       <c r="Z46" s="1">
         <v>5.4166666666666599E-2</v>
@@ -5156,7 +5167,7 @@
       <c r="L47" s="2"/>
       <c r="M47" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45512</v>
+        <v>45514</v>
       </c>
       <c r="N47" s="1">
         <v>8.9583333333333307E-2</v>
@@ -5182,7 +5193,7 @@
       <c r="X47" s="2"/>
       <c r="Y47" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45512</v>
+        <v>45514</v>
       </c>
       <c r="Z47" s="1">
         <v>5.83333333333333E-2</v>
@@ -5226,7 +5237,7 @@
       <c r="L48" s="2"/>
       <c r="M48" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45513</v>
+        <v>45515</v>
       </c>
       <c r="N48" s="1">
         <v>9.1666666666666702E-2</v>
@@ -5252,7 +5263,7 @@
       <c r="X48" s="2"/>
       <c r="Y48" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45513</v>
+        <v>45515</v>
       </c>
       <c r="Z48" s="1">
         <v>6.2499999999999903E-2</v>
@@ -5296,7 +5307,7 @@
       <c r="L49" s="2"/>
       <c r="M49" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45514</v>
+        <v>45516</v>
       </c>
       <c r="N49" s="1">
         <v>9.375E-2</v>
@@ -5322,7 +5333,7 @@
       <c r="X49" s="2"/>
       <c r="Y49" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45514</v>
+        <v>45516</v>
       </c>
       <c r="Z49" s="1">
         <v>6.6666666666666499E-2</v>
@@ -5366,7 +5377,7 @@
       <c r="L50" s="2"/>
       <c r="M50" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45515</v>
+        <v>45517</v>
       </c>
       <c r="N50" s="1">
         <v>9.5833333333333298E-2</v>
@@ -5392,7 +5403,7 @@
       <c r="X50" s="2"/>
       <c r="Y50" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45515</v>
+        <v>45517</v>
       </c>
       <c r="Z50" s="1">
         <v>7.0833333333333207E-2</v>
@@ -5436,7 +5447,7 @@
       <c r="L51" s="2"/>
       <c r="M51" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45516</v>
+        <v>45518</v>
       </c>
       <c r="N51" s="1">
         <v>9.7916666666666693E-2</v>
@@ -5462,7 +5473,7 @@
       <c r="X51" s="2"/>
       <c r="Y51" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45516</v>
+        <v>45518</v>
       </c>
       <c r="Z51" s="1">
         <v>7.4999999999999803E-2</v>
@@ -5506,7 +5517,7 @@
       <c r="L52" s="2"/>
       <c r="M52" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45517</v>
+        <v>45519</v>
       </c>
       <c r="N52" s="1">
         <v>0.1</v>
@@ -5532,7 +5543,7 @@
       <c r="X52" s="2"/>
       <c r="Y52" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45517</v>
+        <v>45519</v>
       </c>
       <c r="Z52" s="1">
         <v>7.9166666666666399E-2</v>
@@ -5576,7 +5587,7 @@
       <c r="L53" s="2"/>
       <c r="M53" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45518</v>
+        <v>45520</v>
       </c>
       <c r="N53" s="1">
         <v>0.102083333333333</v>
@@ -5602,7 +5613,7 @@
       <c r="X53" s="2"/>
       <c r="Y53" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45518</v>
+        <v>45520</v>
       </c>
       <c r="Z53" s="1">
         <v>8.3333333333333107E-2</v>
@@ -5646,7 +5657,7 @@
       <c r="L54" s="2"/>
       <c r="M54" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45519</v>
+        <v>45521</v>
       </c>
       <c r="N54" s="1">
         <v>0.104166666666667</v>
@@ -5672,7 +5683,7 @@
       <c r="X54" s="2"/>
       <c r="Y54" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45519</v>
+        <v>45521</v>
       </c>
       <c r="Z54" s="1">
         <v>9.0277777777777776E-2</v>
@@ -5716,7 +5727,7 @@
       <c r="L55" s="2"/>
       <c r="M55" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45520</v>
+        <v>45522</v>
       </c>
       <c r="N55" s="1">
         <v>0.10625</v>
@@ -5742,7 +5753,7 @@
       <c r="X55" s="2"/>
       <c r="Y55" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45520</v>
+        <v>45522</v>
       </c>
       <c r="Z55" s="1">
         <v>9.7222222222222404E-2</v>
@@ -5786,7 +5797,7 @@
       <c r="L56" s="2"/>
       <c r="M56" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45521</v>
+        <v>45523</v>
       </c>
       <c r="N56" s="1">
         <v>0.108333333333333</v>
@@ -5812,7 +5823,7 @@
       <c r="X56" s="2"/>
       <c r="Y56" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45521</v>
+        <v>45523</v>
       </c>
       <c r="Z56" s="1">
         <v>0.104166666666667</v>
@@ -5856,7 +5867,7 @@
       <c r="L57" s="2"/>
       <c r="M57" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45522</v>
+        <v>45524</v>
       </c>
       <c r="N57" s="1">
         <v>0.110416666666667</v>
@@ -5882,7 +5893,7 @@
       <c r="X57" s="2"/>
       <c r="Y57" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45522</v>
+        <v>45524</v>
       </c>
       <c r="Z57" s="1">
         <v>0.11111111111111199</v>
@@ -5926,7 +5937,7 @@
       <c r="L58" s="2"/>
       <c r="M58" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45523</v>
+        <v>45525</v>
       </c>
       <c r="N58" s="1">
         <v>0.1125</v>
@@ -5952,7 +5963,7 @@
       <c r="X58" s="2"/>
       <c r="Y58" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45523</v>
+        <v>45525</v>
       </c>
       <c r="Z58" s="1">
         <v>0.118055555555556</v>
@@ -5996,7 +6007,7 @@
       <c r="L59" s="2"/>
       <c r="M59" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45524</v>
+        <v>45526</v>
       </c>
       <c r="N59" s="1">
         <v>0.114583333333333</v>
@@ -6022,7 +6033,7 @@
       <c r="X59" s="2"/>
       <c r="Y59" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45524</v>
+        <v>45526</v>
       </c>
       <c r="Z59" s="1">
         <v>0.125000000000001</v>
@@ -6066,7 +6077,7 @@
       <c r="L60" s="2"/>
       <c r="M60" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45525</v>
+        <v>45527</v>
       </c>
       <c r="N60" s="1">
         <v>0.116666666666667</v>
@@ -6092,7 +6103,7 @@
       <c r="X60" s="2"/>
       <c r="Y60" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45525</v>
+        <v>45527</v>
       </c>
       <c r="Z60" s="1">
         <v>0.131944444444446</v>
@@ -6136,7 +6147,7 @@
       <c r="L61" s="2"/>
       <c r="M61" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45526</v>
+        <v>45528</v>
       </c>
       <c r="N61" s="1">
         <v>0.11874999999999999</v>
@@ -6162,7 +6173,7 @@
       <c r="X61" s="2"/>
       <c r="Y61" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45526</v>
+        <v>45528</v>
       </c>
       <c r="Z61" s="1">
         <v>0.138888888888891</v>
@@ -6206,7 +6217,7 @@
       <c r="L62" s="2"/>
       <c r="M62" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45527</v>
+        <v>45529</v>
       </c>
       <c r="N62" s="1">
         <v>0.120833333333333</v>
@@ -6266,7 +6277,7 @@
       <c r="L63" s="2"/>
       <c r="M63" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45528</v>
+        <v>45530</v>
       </c>
       <c r="N63" s="1">
         <v>0.12291666666666699</v>
@@ -6326,7 +6337,7 @@
       <c r="L64" s="2"/>
       <c r="M64" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45529</v>
+        <v>45531</v>
       </c>
       <c r="N64" s="1">
         <v>0.125</v>
@@ -6386,7 +6397,7 @@
       <c r="L65" s="2"/>
       <c r="M65" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45530</v>
+        <v>45532</v>
       </c>
       <c r="N65" s="1">
         <v>0.12708333333333299</v>
@@ -6446,7 +6457,7 @@
       <c r="L66" s="2"/>
       <c r="M66" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45531</v>
+        <v>45533</v>
       </c>
       <c r="N66" s="1">
         <v>0.12916666666666701</v>
@@ -6506,7 +6517,7 @@
       <c r="L67" s="2"/>
       <c r="M67" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45532</v>
+        <v>45534</v>
       </c>
       <c r="N67" s="1">
         <v>0.13125000000000001</v>
@@ -6562,7 +6573,7 @@
       <c r="L68" s="2"/>
       <c r="M68" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45533</v>
+        <v>45535</v>
       </c>
       <c r="N68" s="1">
         <v>0.133333333333333</v>
@@ -6618,7 +6629,7 @@
       <c r="L69" s="2"/>
       <c r="M69" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>45534</v>
+        <v>45536</v>
       </c>
       <c r="N69" s="1">
         <v>0.13541666666666699</v>
@@ -6674,7 +6685,7 @@
       <c r="L70" s="2"/>
       <c r="M70" s="15">
         <f t="shared" ref="M70:M71" ca="1" si="6">M69+1</f>
-        <v>45535</v>
+        <v>45537</v>
       </c>
       <c r="N70" s="1">
         <v>0.13750000000000001</v>
@@ -6730,7 +6741,7 @@
       <c r="L71" s="2"/>
       <c r="M71" s="15">
         <f t="shared" ca="1" si="6"/>
-        <v>45536</v>
+        <v>45538</v>
       </c>
       <c r="N71" s="1">
         <v>0.139583333333333</v>

</xml_diff>

<commit_message>
adding not found page
</commit_message>
<xml_diff>
--- a/track.xlsx
+++ b/track.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\dashboardv.4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2501CC3-999A-4EB1-A47B-430CDBD095E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31A6F665-24BC-4795-B864-940ADD455E1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -1220,9 +1220,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48F4D59D-8EC0-4300-B06F-D1EA277B0BF1}">
   <dimension ref="A1:AJ72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AH18" sqref="AH18"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AH23" sqref="AH23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -1399,11 +1399,11 @@
       <c r="AH2" s="16"/>
       <c r="AI2" s="6">
         <f>(AI3+(AJ3/60))/60</f>
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="AJ2" s="7">
         <f>(AI3+(AJ3/60))</f>
-        <v>45</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.25">
@@ -1521,7 +1521,7 @@
       </c>
       <c r="AI3" s="8">
         <f>SUMIF(Table57[CHECK],"Done",AI$4:AI$71)</f>
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="AJ3" s="8">
         <f>SUMIF(Table57[CHECK],"Done",AJ$4:AJ$71)</f>
@@ -3104,7 +3104,9 @@
       <c r="AG19" s="1">
         <v>3.3333333333333298E-2</v>
       </c>
-      <c r="AH19" s="10"/>
+      <c r="AH19" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="AI19" s="2">
         <v>3</v>
       </c>
@@ -3193,7 +3195,9 @@
       <c r="AG20" s="1">
         <v>3.54166666666667E-2</v>
       </c>
-      <c r="AH20" s="10"/>
+      <c r="AH20" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="AI20" s="2">
         <v>3</v>
       </c>
@@ -3282,7 +3286,9 @@
       <c r="AG21" s="1">
         <v>3.7499999999999999E-2</v>
       </c>
-      <c r="AH21" s="10"/>
+      <c r="AH21" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="AI21" s="2">
         <v>3</v>
       </c>
@@ -3371,7 +3377,9 @@
       <c r="AG22" s="1">
         <v>3.9583333333333401E-2</v>
       </c>
-      <c r="AH22" s="10"/>
+      <c r="AH22" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="AI22" s="2">
         <v>3</v>
       </c>
@@ -3456,7 +3464,9 @@
       <c r="AG23" s="1">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="AH23" s="10"/>
+      <c r="AH23" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="AI23" s="2">
         <v>3</v>
       </c>
@@ -3539,11 +3549,11 @@
         <v>4.1666666666666699E-2</v>
       </c>
       <c r="AG24" s="1">
-        <v>4.3749999999999997E-2</v>
+        <v>4.5833333333333399E-2</v>
       </c>
       <c r="AH24" s="10"/>
       <c r="AI24" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AJ24" s="2">
         <v>0</v>
@@ -3610,14 +3620,14 @@
         <v>45490</v>
       </c>
       <c r="AF25" s="1">
-        <v>4.3749999999999997E-2</v>
+        <v>4.5833333333333399E-2</v>
       </c>
       <c r="AG25" s="1">
-        <v>4.5833333333333399E-2</v>
+        <v>0.05</v>
       </c>
       <c r="AH25" s="10"/>
       <c r="AI25" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AJ25" s="2">
         <v>0</v>
@@ -3684,14 +3694,14 @@
         <v>45491</v>
       </c>
       <c r="AF26" s="1">
-        <v>4.5833333333333302E-2</v>
+        <v>5.00000000000001E-2</v>
       </c>
       <c r="AG26" s="1">
-        <v>4.7916666666666698E-2</v>
+        <v>5.4166666666666599E-2</v>
       </c>
       <c r="AH26" s="10"/>
       <c r="AI26" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AJ26" s="2">
         <v>0</v>
@@ -3758,14 +3768,14 @@
         <v>45492</v>
       </c>
       <c r="AF27" s="1">
-        <v>4.7916666666666698E-2</v>
+        <v>5.41666666666668E-2</v>
       </c>
       <c r="AG27" s="1">
-        <v>0.05</v>
+        <v>5.8333333333333202E-2</v>
       </c>
       <c r="AH27" s="10"/>
       <c r="AI27" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AJ27" s="2">
         <v>0</v>
@@ -3832,14 +3842,14 @@
         <v>45493</v>
       </c>
       <c r="AF28" s="1">
-        <v>0.05</v>
+        <v>5.8333333333333501E-2</v>
       </c>
       <c r="AG28" s="1">
-        <v>5.2083333333333398E-2</v>
+        <v>6.2499999999999799E-2</v>
       </c>
       <c r="AH28" s="10"/>
       <c r="AI28" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AJ28" s="2">
         <v>0</v>
@@ -3906,14 +3916,14 @@
         <v>45494</v>
       </c>
       <c r="AF29" s="1">
-        <v>5.2083333333333301E-2</v>
+        <v>6.2500000000000194E-2</v>
       </c>
       <c r="AG29" s="1">
-        <v>5.4166666666666703E-2</v>
+        <v>6.6666666666666402E-2</v>
       </c>
       <c r="AH29" s="10"/>
       <c r="AI29" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AJ29" s="2">
         <v>0</v>
@@ -3980,14 +3990,14 @@
         <v>45495</v>
       </c>
       <c r="AF30" s="1">
-        <v>5.4166666666666703E-2</v>
+        <v>6.6666666666666902E-2</v>
       </c>
       <c r="AG30" s="1">
-        <v>5.6250000000000099E-2</v>
+        <v>7.0833333333332998E-2</v>
       </c>
       <c r="AH30" s="10"/>
       <c r="AI30" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AJ30" s="2">
         <v>0</v>
@@ -4054,14 +4064,14 @@
         <v>45496</v>
       </c>
       <c r="AF31" s="1">
-        <v>5.6250000000000001E-2</v>
+        <v>7.0833333333333595E-2</v>
       </c>
       <c r="AG31" s="1">
-        <v>5.8333333333333397E-2</v>
+        <v>7.4999999999999595E-2</v>
       </c>
       <c r="AH31" s="10"/>
       <c r="AI31" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AJ31" s="2">
         <v>0</v>
@@ -4128,14 +4138,14 @@
         <v>45497</v>
       </c>
       <c r="AF32" s="1">
-        <v>5.83333333333333E-2</v>
+        <v>7.5000000000000303E-2</v>
       </c>
       <c r="AG32" s="1">
-        <v>6.0416666666666702E-2</v>
+        <v>7.9166666666666205E-2</v>
       </c>
       <c r="AH32" s="10"/>
       <c r="AI32" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AJ32" s="2">
         <v>0</v>
@@ -4202,14 +4212,14 @@
         <v>45498</v>
       </c>
       <c r="AF33" s="1">
-        <v>6.0416666666666702E-2</v>
+        <v>7.9166666666666996E-2</v>
       </c>
       <c r="AG33" s="1">
-        <v>6.2500000000000097E-2</v>
+        <v>8.3333333333332801E-2</v>
       </c>
       <c r="AH33" s="10"/>
       <c r="AI33" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AJ33" s="2">
         <v>0</v>
@@ -4282,9 +4292,7 @@
         <v>6.4583333333333395E-2</v>
       </c>
       <c r="AH34" s="10"/>
-      <c r="AI34" s="2">
-        <v>3</v>
-      </c>
+      <c r="AI34" s="2"/>
       <c r="AJ34" s="2">
         <v>0</v>
       </c>
@@ -4356,9 +4364,7 @@
         <v>6.6666666666666693E-2</v>
       </c>
       <c r="AH35" s="10"/>
-      <c r="AI35" s="2">
-        <v>3</v>
-      </c>
+      <c r="AI35" s="2"/>
       <c r="AJ35" s="2">
         <v>0</v>
       </c>
@@ -4430,9 +4436,7 @@
         <v>6.8750000000000103E-2</v>
       </c>
       <c r="AH36" s="10"/>
-      <c r="AI36" s="2">
-        <v>3</v>
-      </c>
+      <c r="AI36" s="2"/>
       <c r="AJ36" s="2">
         <v>0</v>
       </c>
@@ -4504,9 +4508,7 @@
         <v>7.0833333333333401E-2</v>
       </c>
       <c r="AH37" s="10"/>
-      <c r="AI37" s="2">
-        <v>3</v>
-      </c>
+      <c r="AI37" s="2"/>
       <c r="AJ37" s="2">
         <v>0</v>
       </c>
@@ -4578,9 +4580,7 @@
         <v>7.2916666666666796E-2</v>
       </c>
       <c r="AH38" s="10"/>
-      <c r="AI38" s="2">
-        <v>3</v>
-      </c>
+      <c r="AI38" s="2"/>
       <c r="AJ38" s="2">
         <v>0</v>
       </c>
@@ -4652,9 +4652,7 @@
         <v>7.5000000000000094E-2</v>
       </c>
       <c r="AH39" s="10"/>
-      <c r="AI39" s="2">
-        <v>3</v>
-      </c>
+      <c r="AI39" s="2"/>
       <c r="AJ39" s="2">
         <v>0</v>
       </c>
@@ -4726,9 +4724,7 @@
         <v>7.7083333333333406E-2</v>
       </c>
       <c r="AH40" s="10"/>
-      <c r="AI40" s="2">
-        <v>3</v>
-      </c>
+      <c r="AI40" s="2"/>
       <c r="AJ40" s="2">
         <v>0</v>
       </c>
@@ -4796,9 +4792,7 @@
         <v>7.9166666666666802E-2</v>
       </c>
       <c r="AH41" s="10"/>
-      <c r="AI41" s="2">
-        <v>3</v>
-      </c>
+      <c r="AI41" s="2"/>
       <c r="AJ41" s="2">
         <v>0</v>
       </c>
@@ -4866,9 +4860,7 @@
         <v>8.12500000000001E-2</v>
       </c>
       <c r="AH42" s="10"/>
-      <c r="AI42" s="2">
-        <v>3</v>
-      </c>
+      <c r="AI42" s="2"/>
       <c r="AJ42" s="2">
         <v>0</v>
       </c>
@@ -4936,9 +4928,7 @@
         <v>8.3333333333333398E-2</v>
       </c>
       <c r="AH43" s="10"/>
-      <c r="AI43" s="2">
-        <v>3</v>
-      </c>
+      <c r="AI43" s="2"/>
       <c r="AJ43" s="2">
         <v>0</v>
       </c>
@@ -5006,9 +4996,7 @@
         <v>8.5416666666666793E-2</v>
       </c>
       <c r="AH44" s="10"/>
-      <c r="AI44" s="2">
-        <v>3</v>
-      </c>
+      <c r="AI44" s="2"/>
       <c r="AJ44" s="2">
         <v>0</v>
       </c>
@@ -5076,9 +5064,7 @@
         <v>8.7500000000000105E-2</v>
       </c>
       <c r="AH45" s="10"/>
-      <c r="AI45" s="2">
-        <v>3</v>
-      </c>
+      <c r="AI45" s="2"/>
       <c r="AJ45" s="2">
         <v>0</v>
       </c>
@@ -5146,9 +5132,7 @@
         <v>8.9583333333333404E-2</v>
       </c>
       <c r="AH46" s="10"/>
-      <c r="AI46" s="2">
-        <v>3</v>
-      </c>
+      <c r="AI46" s="2"/>
       <c r="AJ46" s="2">
         <v>0</v>
       </c>
@@ -5216,9 +5200,7 @@
         <v>9.1666666666666799E-2</v>
       </c>
       <c r="AH47" s="10"/>
-      <c r="AI47" s="2">
-        <v>3</v>
-      </c>
+      <c r="AI47" s="2"/>
       <c r="AJ47" s="2">
         <v>0</v>
       </c>
@@ -5286,9 +5268,7 @@
         <v>9.3750000000000097E-2</v>
       </c>
       <c r="AH48" s="10"/>
-      <c r="AI48" s="2">
-        <v>3</v>
-      </c>
+      <c r="AI48" s="2"/>
       <c r="AJ48" s="2">
         <v>0</v>
       </c>
@@ -5356,9 +5336,7 @@
         <v>9.5833333333333506E-2</v>
       </c>
       <c r="AH49" s="10"/>
-      <c r="AI49" s="2">
-        <v>3</v>
-      </c>
+      <c r="AI49" s="2"/>
       <c r="AJ49" s="2">
         <v>0</v>
       </c>
@@ -5426,9 +5404,7 @@
         <v>9.7916666666666805E-2</v>
       </c>
       <c r="AH50" s="10"/>
-      <c r="AI50" s="2">
-        <v>3</v>
-      </c>
+      <c r="AI50" s="2"/>
       <c r="AJ50" s="2">
         <v>0</v>
       </c>
@@ -5496,9 +5472,7 @@
         <v>0.1</v>
       </c>
       <c r="AH51" s="10"/>
-      <c r="AI51" s="2">
-        <v>3</v>
-      </c>
+      <c r="AI51" s="2"/>
       <c r="AJ51" s="2">
         <v>0</v>
       </c>
@@ -5566,9 +5540,7 @@
         <v>0.102083333333333</v>
       </c>
       <c r="AH52" s="10"/>
-      <c r="AI52" s="2">
-        <v>3</v>
-      </c>
+      <c r="AI52" s="2"/>
       <c r="AJ52" s="2">
         <v>0</v>
       </c>
@@ -5636,9 +5608,7 @@
         <v>0.10416666666666601</v>
       </c>
       <c r="AH53" s="10"/>
-      <c r="AI53" s="2">
-        <v>3</v>
-      </c>
+      <c r="AI53" s="2"/>
       <c r="AJ53" s="2">
         <v>0</v>
       </c>
@@ -5706,9 +5676,7 @@
         <v>0.10625</v>
       </c>
       <c r="AH54" s="10"/>
-      <c r="AI54" s="2">
-        <v>3</v>
-      </c>
+      <c r="AI54" s="2"/>
       <c r="AJ54" s="2">
         <v>0</v>
       </c>
@@ -5776,9 +5744,7 @@
         <v>0.108333333333333</v>
       </c>
       <c r="AH55" s="10"/>
-      <c r="AI55" s="2">
-        <v>3</v>
-      </c>
+      <c r="AI55" s="2"/>
       <c r="AJ55" s="2">
         <v>0</v>
       </c>
@@ -5846,9 +5812,7 @@
         <v>0.110416666666667</v>
       </c>
       <c r="AH56" s="10"/>
-      <c r="AI56" s="2">
-        <v>3</v>
-      </c>
+      <c r="AI56" s="2"/>
       <c r="AJ56" s="2">
         <v>0</v>
       </c>
@@ -5916,9 +5880,7 @@
         <v>0.1125</v>
       </c>
       <c r="AH57" s="10"/>
-      <c r="AI57" s="2">
-        <v>3</v>
-      </c>
+      <c r="AI57" s="2"/>
       <c r="AJ57" s="2">
         <v>0</v>
       </c>
@@ -5986,9 +5948,7 @@
         <v>0.114583333333333</v>
       </c>
       <c r="AH58" s="10"/>
-      <c r="AI58" s="2">
-        <v>3</v>
-      </c>
+      <c r="AI58" s="2"/>
       <c r="AJ58" s="2">
         <v>0</v>
       </c>
@@ -6056,9 +6016,7 @@
         <v>0.116666666666667</v>
       </c>
       <c r="AH59" s="10"/>
-      <c r="AI59" s="2">
-        <v>3</v>
-      </c>
+      <c r="AI59" s="2"/>
       <c r="AJ59" s="2">
         <v>0</v>
       </c>
@@ -6126,9 +6084,7 @@
         <v>0.11874999999999999</v>
       </c>
       <c r="AH60" s="10"/>
-      <c r="AI60" s="2">
-        <v>3</v>
-      </c>
+      <c r="AI60" s="2"/>
       <c r="AJ60" s="2">
         <v>0</v>
       </c>
@@ -6196,9 +6152,7 @@
         <v>0.120833333333333</v>
       </c>
       <c r="AH61" s="10"/>
-      <c r="AI61" s="2">
-        <v>3</v>
-      </c>
+      <c r="AI61" s="2"/>
       <c r="AJ61" s="2">
         <v>0</v>
       </c>
@@ -6256,9 +6210,7 @@
         <v>0.12291666666666699</v>
       </c>
       <c r="AH62" s="10"/>
-      <c r="AI62" s="2">
-        <v>3</v>
-      </c>
+      <c r="AI62" s="2"/>
       <c r="AJ62" s="2">
         <v>0</v>
       </c>
@@ -6316,9 +6268,7 @@
         <v>0.125</v>
       </c>
       <c r="AH63" s="10"/>
-      <c r="AI63" s="2">
-        <v>3</v>
-      </c>
+      <c r="AI63" s="2"/>
       <c r="AJ63" s="2">
         <v>0</v>
       </c>
@@ -6376,9 +6326,7 @@
         <v>0.12708333333333299</v>
       </c>
       <c r="AH64" s="10"/>
-      <c r="AI64" s="2">
-        <v>3</v>
-      </c>
+      <c r="AI64" s="2"/>
       <c r="AJ64" s="2">
         <v>0</v>
       </c>
@@ -6436,9 +6384,7 @@
         <v>0.12916666666666701</v>
       </c>
       <c r="AH65" s="10"/>
-      <c r="AI65" s="2">
-        <v>3</v>
-      </c>
+      <c r="AI65" s="2"/>
       <c r="AJ65" s="2">
         <v>0</v>
       </c>
@@ -6496,9 +6442,7 @@
         <v>0.13125000000000001</v>
       </c>
       <c r="AH66" s="10"/>
-      <c r="AI66" s="2">
-        <v>3</v>
-      </c>
+      <c r="AI66" s="2"/>
       <c r="AJ66" s="2">
         <v>0</v>
       </c>
@@ -6552,9 +6496,7 @@
       <c r="AF67" s="1"/>
       <c r="AG67" s="1"/>
       <c r="AH67" s="10"/>
-      <c r="AI67" s="2">
-        <v>3</v>
-      </c>
+      <c r="AI67" s="2"/>
       <c r="AJ67" s="2">
         <v>0</v>
       </c>
@@ -6608,9 +6550,7 @@
       <c r="AF68" s="1"/>
       <c r="AG68" s="1"/>
       <c r="AH68" s="10"/>
-      <c r="AI68" s="2">
-        <v>3</v>
-      </c>
+      <c r="AI68" s="2"/>
       <c r="AJ68" s="2">
         <v>0</v>
       </c>
@@ -6664,9 +6604,7 @@
       <c r="AF69" s="1"/>
       <c r="AG69" s="1"/>
       <c r="AH69" s="10"/>
-      <c r="AI69" s="2">
-        <v>3</v>
-      </c>
+      <c r="AI69" s="2"/>
       <c r="AJ69" s="2">
         <v>0</v>
       </c>
@@ -6720,9 +6658,7 @@
       <c r="AF70" s="1"/>
       <c r="AG70" s="1"/>
       <c r="AH70" s="10"/>
-      <c r="AI70" s="2">
-        <v>3</v>
-      </c>
+      <c r="AI70" s="2"/>
       <c r="AJ70" s="2">
         <v>0</v>
       </c>
@@ -6776,9 +6712,7 @@
       <c r="AF71" s="1"/>
       <c r="AG71" s="1"/>
       <c r="AH71" s="10"/>
-      <c r="AI71" s="2">
-        <v>3</v>
-      </c>
+      <c r="AI71" s="2"/>
       <c r="AJ71" s="2">
         <v>0</v>
       </c>

</xml_diff>